<commit_message>
fix dates in fit_sitemgmt
</commit_message>
<xml_diff>
--- a/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
+++ b/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="56">
   <si>
     <t>reps_nu</t>
   </si>
@@ -173,118 +173,33 @@
     <t>sampled2019</t>
   </si>
   <si>
-    <r>
-      <t>April 15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-Roundup Powermax 32 oz; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>April 15-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Acetochlor ATZ 40 oz; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>May 14-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Aatrex 9-0   1/2; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>May 14-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Harness Max  40 oz; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>June 15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">-Warrant Ultra 50 oz; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>June 15-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>Roundup Powermax 22 oz;</t>
-    </r>
+    <t>April 15-Roundup Powermax 32 oz; April 15-Acetochlor ATZ 40 oz; May 14-Aatrex 9-0   1/2; May 14-Harness Max  40 oz; June 15-Warrant Ultra 50 oz; June 15-Roundup Powermax 22 oz;</t>
+  </si>
+  <si>
+    <t>15-Apr</t>
+  </si>
+  <si>
+    <t>25-Apr</t>
+  </si>
+  <si>
+    <t>1-May</t>
+  </si>
+  <si>
+    <t>5-May</t>
+  </si>
+  <si>
+    <t>10-May</t>
+  </si>
+  <si>
+    <t>26-Apr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -316,12 +231,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Symbol"/>
       <family val="1"/>
@@ -348,52 +257,49 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,455 +584,465 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="32.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="4" customWidth="1"/>
-    <col min="6" max="7" width="9.140625" style="4"/>
-    <col min="8" max="8" width="64.140625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="13.140625" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="15.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="3" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="3"/>
+    <col min="8" max="8" width="64.140625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="13.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="13.140625" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="105" x14ac:dyDescent="0.25">
-      <c r="H1" s="4" t="s">
+      <c r="A1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="10"/>
+      <c r="K1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="O2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="10" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="4">
         <v>2009</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="10">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="5" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="2">
-        <v>43570</v>
-      </c>
-      <c r="M3" s="5">
-        <v>43581</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="L3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="N3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="6">
         <v>2009</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="6">
         <v>5</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="J4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L4" s="11">
-        <v>43580</v>
-      </c>
-      <c r="M4" s="12">
-        <v>43590</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="L4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="4" t="s">
+      <c r="O4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P4" s="4" t="s">
+      <c r="P4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="6">
         <v>2002</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="11">
-        <v>43570</v>
-      </c>
-      <c r="M5" s="12">
-        <v>43581</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="L5" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="N5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="P5" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="6">
         <v>2002</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="6">
         <v>5</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="11">
-        <v>43580</v>
-      </c>
-      <c r="M6" s="12">
-        <v>43590</v>
-      </c>
-      <c r="N6" s="4" t="s">
+      <c r="L6" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="P6" s="4" t="s">
+      <c r="P6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>2008</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="6">
         <v>4</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="L7" s="12">
-        <v>43952</v>
-      </c>
-      <c r="M7" s="12">
-        <v>43595</v>
-      </c>
-      <c r="N7" s="4" t="s">
+      <c r="L7" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="P7" s="4" t="s">
+      <c r="P7" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>2009</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="6">
         <v>4</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="H8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="12">
-        <v>43952</v>
-      </c>
-      <c r="M8" s="12">
-        <v>43590</v>
-      </c>
-      <c r="N8" s="4" t="s">
+      <c r="L8" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="10" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="15"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="15"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="H13" s="3"/>
+      <c r="H13" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix site mgmt to have active ing, add pfi_herbicidekey
</commit_message>
<xml_diff>
--- a/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
+++ b/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
@@ -56,9 +56,6 @@
     <t>herb_fall2018</t>
   </si>
   <si>
-    <t>glyphosate 1 week before corn planting, Lumax at planting</t>
-  </si>
-  <si>
     <t>glyphosate 1 week before soybean planting</t>
   </si>
   <si>
@@ -155,12 +152,6 @@
     <t>herb_spring2019</t>
   </si>
   <si>
-    <t>Roundup and Cadet</t>
-  </si>
-  <si>
-    <t>3 oz Fierce XLT  with 26-32 oz Roundup Powermax as burndown followed by a post emergence application of 22 oz Xtendimax plus 2 pt of Warrant</t>
-  </si>
-  <si>
     <t>liquid swine, ~3000 gal/ac every other year to entire field</t>
   </si>
   <si>
@@ -173,9 +164,6 @@
     <t>sampled2019</t>
   </si>
   <si>
-    <t>April 15-Roundup Powermax 32 oz; April 15-Acetochlor ATZ 40 oz; May 14-Aatrex 9-0   1/2; May 14-Harness Max  40 oz; June 15-Warrant Ultra 50 oz; June 15-Roundup Powermax 22 oz;</t>
-  </si>
-  <si>
     <t>15-Apr</t>
   </si>
   <si>
@@ -192,6 +180,18 @@
   </si>
   <si>
     <t>26-Apr</t>
+  </si>
+  <si>
+    <t>glyphosate 1 week before maize planting; metalochlor, atrazine, and mesotrione at planting</t>
+  </si>
+  <si>
+    <t>glyphosate before planting; glyphosate and fluthiacet-methyl at planting</t>
+  </si>
+  <si>
+    <t>glyphosate and acetochlor  before planting (April 15), atrazine, acetochlor at planting (May 14); acetochlor and glyphosate after planting (June 15)</t>
+  </si>
+  <si>
+    <t>chlorimuron-ethyl, flumioxazin, pyroxasulfone, and glyphosate before planting, dicamba and acetochlor after planting</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,30 +610,30 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
       <c r="H1" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" s="10"/>
       <c r="K1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="10" t="s">
         <v>22</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>23</v>
       </c>
       <c r="N1" s="10"/>
       <c r="O1" s="10"/>
       <c r="P1" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>1</v>
@@ -642,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>5</v>
@@ -651,42 +651,42 @@
         <v>0</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M2" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="N2" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>3</v>
@@ -701,31 +701,31 @@
         <v>5</v>
       </c>
       <c r="G3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O3" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="P3" s="10" t="s">
         <v>4</v>
@@ -733,10 +733,10 @@
     </row>
     <row r="4" spans="1:16" ht="51" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -751,45 +751,45 @@
         <v>5</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O4" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="P4" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="63.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>27</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>28</v>
       </c>
       <c r="D5" s="6">
         <v>2002</v>
@@ -801,31 +801,31 @@
         <v>5</v>
       </c>
       <c r="G5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="M5" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O5" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="H5" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="M5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="P5" s="10" t="s">
         <v>4</v>
@@ -833,13 +833,13 @@
     </row>
     <row r="6" spans="1:16" ht="51" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="6">
         <v>2002</v>
@@ -854,39 +854,39 @@
         <v>4</v>
       </c>
       <c r="H6" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>11</v>
-      </c>
       <c r="K6" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="N6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>14</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>15</v>
       </c>
       <c r="P6" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
@@ -901,31 +901,31 @@
         <v>4</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="K7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="N7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="O7" s="10" t="s">
         <v>39</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="N7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="O7" s="10" t="s">
-        <v>40</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>4</v>
@@ -933,10 +933,10 @@
     </row>
     <row r="8" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>3</v>
@@ -945,37 +945,37 @@
         <v>2009</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6">
         <v>4</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>53</v>
-      </c>
       <c r="N8" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
make chicken or turkey instead of backslash
</commit_message>
<xml_diff>
--- a/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
+++ b/data-raw/pfi_sitemgmt/PFIweeds_site_summaries-nice.xlsx
@@ -143,9 +143,6 @@
     <t>burndown, pre-emergent herbicide</t>
   </si>
   <si>
-    <t>chicken/turkey manure</t>
-  </si>
-  <si>
     <t>tillage</t>
   </si>
   <si>
@@ -192,6 +189,9 @@
   </si>
   <si>
     <t>chlorimuron-ethyl, flumioxazin, pyroxasulfone, and glyphosate before planting, dicamba and acetochlor after planting</t>
+  </si>
+  <si>
+    <t>chicken or turkey manure</t>
   </si>
 </sst>
 </file>
@@ -584,7 +584,7 @@
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H2" s="10" t="s">
         <v>35</v>
@@ -660,7 +660,7 @@
         <v>9</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>11</v>
@@ -672,13 +672,13 @@
         <v>17</v>
       </c>
       <c r="N2" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="O2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P2" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="89.25" x14ac:dyDescent="0.25">
@@ -710,16 +710,16 @@
         <v>28</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>36</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N3" s="10" t="s">
         <v>13</v>
@@ -754,7 +754,7 @@
         <v>13</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="7" t="s">
         <v>28</v>
@@ -766,10 +766,10 @@
         <v>36</v>
       </c>
       <c r="L4" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M4" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>13</v>
@@ -810,16 +810,16 @@
         <v>28</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N5" s="10" t="s">
         <v>13</v>
@@ -854,7 +854,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>28</v>
@@ -866,10 +866,10 @@
         <v>36</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N6" s="10" t="s">
         <v>13</v>
@@ -904,28 +904,28 @@
         <v>13</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I7" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J7" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K7" s="6" t="s">
         <v>38</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>13</v>
       </c>
       <c r="O7" s="10" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="P7" s="10" t="s">
         <v>4</v>
@@ -954,28 +954,28 @@
         <v>13</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="L8" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>48</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>49</v>
       </c>
       <c r="N8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="O8" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P8" s="10" t="s">
         <v>4</v>

</xml_diff>